<commit_message>
Comment about bootstrap added
</commit_message>
<xml_diff>
--- a/Folders description.xlsx
+++ b/Folders description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/svegas/Sira/Sira/Publicaciones/Revistas/EMSE Percepciones/Final/Misperceptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F68CF59-37EA-6D40-B577-DCFB76F8DB4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7780E20C-7BD6-BD4B-95B6-4F1C8E5CCFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1020" windowWidth="26020" windowHeight="16380" xr2:uid="{C544198C-A2E8-DF47-84CF-FEB3C7D22882}"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="26020" windowHeight="16380" activeTab="1" xr2:uid="{C544198C-A2E8-DF47-84CF-FEB3C7D22882}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Study" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="89">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -74,9 +74,6 @@
     <t>RQ1.2 Stuart-Maxwell.xlsx</t>
   </si>
   <si>
-    <t>Contingency tables in RQ1.2 Kappa.spv</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Original Experiment analysis/Original Experiment data.sav</t>
   </si>
   <si>
-    <t>AICs in All mixed models OE.sps</t>
-  </si>
-  <si>
     <t>Results in Best model OE.sps</t>
   </si>
   <si>
@@ -159,6 +153,154 @@
   </si>
   <si>
     <t>Data all techniques.sav</t>
+  </si>
+  <si>
+    <t>COMMENTS</t>
+  </si>
+  <si>
+    <t>Alpha's confidence intervals have been calculated with bootstrap. Bounds might vary slightly when analyses are re-run</t>
+  </si>
+  <si>
+    <t>Kappa's confidence intervals have been calculated with bootstrap. Bounds might vary slightly when analyses are re-run</t>
+  </si>
+  <si>
+    <t>Replicated Experiment analysis/Replicated Experiment.sav</t>
+  </si>
+  <si>
+    <t>Replicated Experiment analysis/All mixed models RE.spv</t>
+  </si>
+  <si>
+    <t>Replicated Experiment analysis/Best model RE.spv</t>
+  </si>
+  <si>
+    <t>Replicated Experiment analysis/Model selection RE.xlsx</t>
+  </si>
+  <si>
+    <t>AICs in file: All mixed models RE.sps</t>
+  </si>
+  <si>
+    <t>AICs in file: All mixed models OE.sps</t>
+  </si>
+  <si>
+    <t>Replicated Experiment analysis/All mixed models RE.sps</t>
+  </si>
+  <si>
+    <t>Replicated Experiment analysis/Best model RE.sps</t>
+  </si>
+  <si>
+    <t>RQ2.1.spv</t>
+  </si>
+  <si>
+    <t>RQ1.6 Kappa.spv</t>
+  </si>
+  <si>
+    <t>RQ1.6 McNemar-Bowker.spv</t>
+  </si>
+  <si>
+    <t>RQ1.6 Stuart-Maxwell.xlsx</t>
+  </si>
+  <si>
+    <t>Results of Kappa for RQ1.6</t>
+  </si>
+  <si>
+    <t>Results of McNemar-Bowker test for RQ1.6</t>
+  </si>
+  <si>
+    <t>Results of Stuart-Maxwell test for RQ1.6</t>
+  </si>
+  <si>
+    <t>Contingency tables in file: RQ1.6 Kappa.spv</t>
+  </si>
+  <si>
+    <t>Contingency tables in file: RQ1.2 Kappa.spv</t>
+  </si>
+  <si>
+    <t>RQ2.2 Kappa.spv</t>
+  </si>
+  <si>
+    <t>RQ2.2 McNemar-Bowker.spv</t>
+  </si>
+  <si>
+    <t>RQ2.2 Stuart-Maxwell.xlsx</t>
+  </si>
+  <si>
+    <t>RQ3.1 Kappa.spv</t>
+  </si>
+  <si>
+    <t>RQ3.1 McNemar-Bowker.spv</t>
+  </si>
+  <si>
+    <t>RQ3.1 Stuart-Maxwell.xlsx</t>
+  </si>
+  <si>
+    <t>RQ3.2 Kappa.spv</t>
+  </si>
+  <si>
+    <t>Data Programs RS.sav
+Data Techniques RS.sav</t>
+  </si>
+  <si>
+    <t>Data Techniques RS.sav</t>
+  </si>
+  <si>
+    <t>Contingency tables for techniques in file: RQ1.2 Kappa.spv</t>
+  </si>
+  <si>
+    <t>Data Techiques RS.sav</t>
+  </si>
+  <si>
+    <t>Results of chi-square goodness-of-fit for RQ2.1</t>
+  </si>
+  <si>
+    <t>RQ2.1sps</t>
+  </si>
+  <si>
+    <t>RQ2.2 Kappa.sps</t>
+  </si>
+  <si>
+    <t>RQ2.2 McNemar-Bowker.sps</t>
+  </si>
+  <si>
+    <t>Contingency tables in file: RQ2.2 Kappa.spv</t>
+  </si>
+  <si>
+    <t>Results of McNemar-Bowker test for RQ2.2</t>
+  </si>
+  <si>
+    <t>Results of Stuart-Maxwell test for RQ2.2</t>
+  </si>
+  <si>
+    <t>Results of Kappa for RQ2.2</t>
+  </si>
+  <si>
+    <t>RQ1.6 Kappa.sps</t>
+  </si>
+  <si>
+    <t>RQ1.6 McNemar-Bowker.sps</t>
+  </si>
+  <si>
+    <t>RQ3.1 Kappa.sps</t>
+  </si>
+  <si>
+    <t>RQ3.1 McNemar-Bowker.sps</t>
+  </si>
+  <si>
+    <t>RQ3.2 Kappa.sps</t>
+  </si>
+  <si>
+    <t>Results of Kappa for RQ3.2</t>
+  </si>
+  <si>
+    <t>Results of Stuart-Maxwell test for RQ3.1</t>
+  </si>
+  <si>
+    <t>Results of McNemar-Bowker test for RQ3.1</t>
+  </si>
+  <si>
+    <t>Results of Kappa for RQ3.1</t>
+  </si>
+  <si>
+    <t>Contingency tables in file: RQ3.1 Kappa.spv</t>
   </si>
 </sst>
 </file>
@@ -215,15 +357,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511C6610-876D-C347-B7E3-61FBC9E1525C}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,180 +695,190 @@
     <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -737,22 +892,368 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53E9868-F8D1-D14B-973A-15C941CCC417}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24187AD6-6A7C-B74E-BF1D-7620046D7F14}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,124 +1262,135 @@
     <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>